<commit_message>
fixed figs for final review
</commit_message>
<xml_diff>
--- a/data_stefan/trt_mgmt.Abels.ReduceN.xlsx
+++ b/data_stefan/trt_mgmt.Abels.ReduceN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://practicalfarmers.sharepoint.com/sites/Research/Shared Documents/CooperatorsProgram/ResearchProjects/FieldCrops/2022-2024/Can We Reduce N Rates and Improve ROI/2023/Cooperators/Fred Abels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\PFI_CanWeReduceN2\data_stefan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="8_{401F9AEE-7283-4C01-86BF-3A32F4D64FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B5C819-E314-4C5A-975D-3F4149EEF5E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23093B94-CB2D-4320-B43B-6F8E30C621D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BA11CEDC-CF96-4B69-AD2E-31C9B22CE6DC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BA11CEDC-CF96-4B69-AD2E-31C9B22CE6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
+  <si>
+    <t>trial_key</t>
+  </si>
   <si>
     <t>first_name</t>
   </si>
@@ -58,6 +61,9 @@
     <t>zipcode</t>
   </si>
   <si>
+    <t>abel_23</t>
+  </si>
+  <si>
     <t>Fred</t>
   </si>
   <si>
@@ -310,12 +316,54 @@
     <t>sidedress</t>
   </si>
   <si>
+    <t>Nrate</t>
+  </si>
+  <si>
     <t>rep</t>
   </si>
   <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
     <t>Details</t>
   </si>
   <si>
+    <t>Cash or forage crop</t>
+  </si>
+  <si>
+    <t>soybeans</t>
+  </si>
+  <si>
+    <t>Tillage</t>
+  </si>
+  <si>
+    <t>no till</t>
+  </si>
+  <si>
+    <t>Manure or compost application intended for cash or forage crop</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>List any cover crops seeded during the year</t>
+  </si>
+  <si>
+    <t>cereal rye</t>
+  </si>
+  <si>
+    <t>Describe any grazing that occurred in the field</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
     <t>Number of replicates (total number of strips divided by 2)</t>
   </si>
   <si>
@@ -328,9 +376,6 @@
     <t>Previous cash crop</t>
   </si>
   <si>
-    <t>soybeans</t>
-  </si>
-  <si>
     <t>Field name</t>
   </si>
   <si>
@@ -346,9 +391,6 @@
     <t>Cover crop type</t>
   </si>
   <si>
-    <t>cereal rye</t>
-  </si>
-  <si>
     <t>cereal rye 150#'s, drill,10" rows</t>
   </si>
   <si>
@@ -395,48 +437,6 @@
   </si>
   <si>
     <t>Observations</t>
-  </si>
-  <si>
-    <t>trial_key</t>
-  </si>
-  <si>
-    <t>abel_23</t>
-  </si>
-  <si>
-    <t>Nrate</t>
-  </si>
-  <si>
-    <t>yield</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Cash or forage crop</t>
-  </si>
-  <si>
-    <t>Tillage</t>
-  </si>
-  <si>
-    <t>no till</t>
-  </si>
-  <si>
-    <t>Manure or compost application intended for cash or forage crop</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>List any cover crops seeded during the year</t>
-  </si>
-  <si>
-    <t>Describe any grazing that occurred in the field</t>
-  </si>
-  <si>
-    <t>corn</t>
   </si>
 </sst>
 </file>
@@ -576,9 +576,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -616,7 +616,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -722,7 +722,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -864,7 +864,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -875,47 +875,47 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>50642</v>
@@ -932,167 +932,167 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C1" s="12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="8">
         <v>45042</v>
@@ -1101,123 +1101,123 @@
         <v>45042</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" s="7">
-        <v>60</v>
+        <v>38.5</v>
       </c>
       <c r="D15" s="7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="7">
-        <v>90</v>
-      </c>
-      <c r="D22" s="7">
+        <v>59</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C23" s="8">
         <v>45092</v>
@@ -1226,27 +1226,27 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="7">
         <v>116.5</v>
@@ -1255,12 +1255,12 @@
         <v>81.5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C26" s="7">
         <v>0.9375</v>
@@ -1269,52 +1269,52 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1329,160 +1329,160 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DC56BD-9148-4794-92ED-92DA1FAA7822}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E2" s="8">
         <v>45042</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G2" s="7">
-        <v>60</v>
+        <v>38.5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E3" s="8">
         <v>45042</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G3" s="7">
-        <v>60</v>
+        <v>38.5</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E4" s="8">
         <v>45092</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G4" s="7">
-        <v>90</v>
+        <v>116.5</v>
       </c>
       <c r="H4" s="7">
         <v>0.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E5" s="8">
         <v>45092</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G5" s="7">
-        <v>60</v>
+        <v>81.5</v>
       </c>
       <c r="H5" s="7">
         <v>0.9375</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E7" s="8"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1502,25 +1502,25 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4">
         <v>150</v>
@@ -1532,9 +1532,9 @@
         <v>166.9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4">
         <v>120</v>
@@ -1546,9 +1546,9 @@
         <v>189.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" s="4">
         <v>120</v>
@@ -1560,9 +1560,9 @@
         <v>190.9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B5" s="4">
         <v>150</v>
@@ -1574,9 +1574,9 @@
         <v>184.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4">
         <v>120</v>
@@ -1588,9 +1588,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B7" s="4">
         <v>150</v>
@@ -1602,9 +1602,9 @@
         <v>182.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" s="4">
         <v>150</v>
@@ -1616,9 +1616,9 @@
         <v>175.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B9" s="4">
         <v>120</v>
@@ -1644,350 +1644,350 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B2" s="4">
         <v>2018</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B3" s="4">
         <v>2018</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4">
         <v>2018</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4">
         <v>2018</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B6" s="4">
         <v>2018</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B7" s="4">
         <v>2019</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B8" s="4">
         <v>2019</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B9" s="4">
         <v>2019</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B10" s="4">
         <v>2019</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B11" s="4">
         <v>2019</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B12" s="4">
         <v>2020</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B13" s="4">
         <v>2020</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B14" s="4">
         <v>2020</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B15" s="4">
         <v>2020</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4">
         <v>2020</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B17" s="4">
         <v>2021</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B18" s="4">
         <v>2021</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B19" s="4">
         <v>2021</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B20" s="4">
         <v>2021</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B21" s="4">
         <v>2021</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B22" s="4">
         <v>2022</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B23" s="4">
         <v>2022</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B24" s="4">
         <v>2022</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B25" s="4">
         <v>2022</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B26" s="4">
         <v>2022</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B27" s="4">
         <v>2023</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B28" s="4">
         <v>2023</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B29" s="4">
         <v>2023</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B30" s="4">
         <v>2023</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B31" s="4">
         <v>2023</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2004,223 +2004,223 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.81640625" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C1" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B2" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B3" s="7">
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B4" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B7" s="7">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B11" s="8">
         <v>44854</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B12" s="8">
         <v>45041</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B15" s="8">
         <v>45064</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B16" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B17" s="7">
         <v>36000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B18" s="8">
         <v>45236</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B19" s="16">
         <v>4.54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="4"/>
@@ -2496,20 +2496,29 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56253EEC-E66A-436A-B529-C957B1E9FD22}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="5c162411-790a-4090-8516-4c29411b79ed"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="170271cd-7847-44f3-81b8-91d966c9299e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE58DB7C-77FF-4661-83CF-F6A7539D9E8B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE58DB7C-77FF-4661-83CF-F6A7539D9E8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="170271cd-7847-44f3-81b8-91d966c9299e"/>
+    <ds:schemaRef ds:uri="5c162411-790a-4090-8516-4c29411b79ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>